<commit_message>
Adiciona venv/ ao .gitignore para excluir da versão
</commit_message>
<xml_diff>
--- a/arquivos/resultados/saida_controle_atualizada.xlsx
+++ b/arquivos/resultados/saida_controle_atualizada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,187 +472,325 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>72.857</v>
+        <v>72.791</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CALUMA RESTAURANTE LTDA (CALUMA BUFFET E REST.)</t>
+          <t>MASTER MEATS (BOUTIQUE DE CARNES)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Avenida das Nações Unidas, 12901, LOJA 123/124 - Brooklin Paulista São Paulo/SP CEP:04578000</t>
+          <t>Rua Abílio Soares, 731 - Paraíso São Paulo/SP CEP:04005003</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>72.858</v>
+        <v>72.83799999999999</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>JESSICA ELAYNE OLIVEIRA DA SILVA (BURGUESA HAMBURGUERIA ARTESANAL)</t>
+          <t>MYW1 O BAR LTDA (VASSOURA QUEBRADA - PERDIZES)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Rua dos Jornalistas, 68, APTO 12 - Cidade Vargas São Paulo/SP CEP:04318-000</t>
+          <t>Rua Desembargador do Vale, 836, ANEXO 830 - Perdizes São Paulo/SP CEP:05010040</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>72.86499999999999</v>
+        <v>72.85899999999999</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>JOYCE REGINA UEDA FERNANDES (JOY PORKARIA'S)</t>
+          <t>MRL BUS COM. DE ALIM. EIRELI - ME (BUSGER - VILA MADALENA)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Avenida Celso dos Santos, 991 - Vila Constança São Paulo/SP CEP:04658241</t>
+          <t>Rua Alves Guimarães, 1091, COZINHA 4 - Pinheiros São Paulo/SP CEP:05410-002</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>72.869</v>
+        <v>72.89100000000001</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>HOTEL MARCO INTERNACIONAL S.A. (PANINI - CID. JARDIM)</t>
+          <t>ECULLY CHARBON RESTAURANTE LTDA (ECULLY CHARBON)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>AVENIDA MAGALHAES DE CASTRO, 12000, SALÃO COMERCIAL LOJA 17/18.3 PISO 3 - CIDADE JARDIM São Paulo/SP CEP:05676-120</t>
+          <t>Rua Doutor Augusto de Miranda, 549 - Vila Pompéia São Paulo/SP CEP:05026000</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>72.91200000000001</v>
+        <v>72.90300000000001</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>BR CORPORE REST. LANCH. IMC LTDA (I LOVE BURGER - BR CORPORE)</t>
+          <t>BAR &amp; REST PICANHARIA DOS AMIGOS LTDA (PICANHARIA DOS AMIGOS - VILA LEOPOLDINA)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Rua Capitão Otávio Machado, 994 - Chácara Santo Antônio (Zona Sul) São Paulo/SP CEP:04718002</t>
+          <t>Rua Guaipá, 1017,  - Vila Leopoldina São Paulo/SP CEP:05089-001</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>72.913</v>
+        <v>72.935</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>BR COMPANY REST. LANCH. LTDA ME (I LOVE BURGER - BR COMPANY)</t>
+          <t>CAPITAO COM. E DIST. BEBIDAS E ALIMENTOS (CAPITAO BARLEY)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Rua Amador Bueno, 767, LOJA I LOVE BURGER  - Santo Amaro São Paulo/SP CEP:04752005</t>
+          <t>Rua Coriolano, 301 - Vila Romana São Paulo/SP CEP:05047001</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>72.92700000000001</v>
+        <v>72.937</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ANNE SUELEM FARIAS MAGAVE PICANCO BEZERRA (DIDIOS BURGER)</t>
+          <t>PARCEL SW BURGUER LTDA (N! BURGER - LAPA)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Rua Maria Virgínia Estensoro, 40, BLOCO A - Jardim da Pedreira São Paulo/SP CEP:04462-080</t>
+          <t>Rua Catão, 479, NBURGER - Vila Romana São Paulo/SP CEP:05049000</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>72.928</v>
+        <v>72.941</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>MARIA JOSE FATIMA DA SILVA CIRINO (MONSTER BURGUER)</t>
+          <t>TOSQUINHO LANCHES LTDA (TOSQUINHO LANCHES)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Rua Estampa Esportiva, 508,  - Americanópolis São Paulo/SP CEP:04429-060</t>
+          <t>RUA CAMILO, 763, sem complemento - VILA ROMANA São Paulo/SP CEP:05045020</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>72.956</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>*CLIENTE AMOSTRA (CLIENTE AMOSTRA)*</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Rua José Mariano Filho, 200,  - Jardim Oriental São Paulo/SP CEP:04347-180</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>72.967</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>GILBERTO CAMPOS DE AZAMBUJA ME (ROYAL MEAT - PARAISO)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Rua Doutor Tomás Carvalhal, 626 - Paraíso São Paulo/SP CEP:04006001</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>72.97</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>THE BEAR BURGER REST. LTDA EPP (THE BEAR BURGER)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Rua Caraíbas, 964, IMOBILIARIA ESTEVAM - Perdizes São Paulo/SP CEP:05020000</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>72.988</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>BUSGER COM. DE ALIM. LTDA (BUSGER - KLABIN)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Rua Vergueiro, 4289,  - Vila Mariana São Paulo/SP CEP:04101-901</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>30</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>72.98999999999999</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>ESTEFOODS COM. DE ALIMENTOS LTDA (BUSGER - BORGES LAGOA)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Rua Borges Lagoa, 1050,  - Vila Clementino São Paulo/SP CEP:04038-002</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>26</v>
+      </c>
+      <c r="G14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>73.008</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>BORGER BURGER LTDA (BORGER - PERDIZES)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Rua Cardoso de Almeida, 587,  - Perdizes São Paulo/SP CEP:05013-000</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>